<commit_message>
Avance reporte de actividades y metas
</commit_message>
<xml_diff>
--- a/docs/Actividades y Metas/tabla_dependencias_actividad_meta.xlsx
+++ b/docs/Actividades y Metas/tabla_dependencias_actividad_meta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_720\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git\repos\00078-DWeb_GestionPlanillas\docs\Actividades y Metas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9D1983C-A724-4150-B95F-5931D631EAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82066324-D312-4FF1-833D-4FE52DA51F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabla_dependencias_actividad_me" sheetId="1" r:id="rId1"/>
@@ -537,7 +537,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -660,7 +660,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -956,26 +956,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F99" sqref="F99"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="79.28515625" customWidth="1"/>
+    <col min="3" max="3" width="53.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="6.140625" customWidth="1"/>
-    <col min="6" max="6" width="68.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
     <col min="7" max="7" width="28.7109375" customWidth="1"/>
-    <col min="8" max="8" width="68.7109375" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
     <col min="9" max="256" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1026,8 +1024,12 @@
       <c r="H2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" t="str">
+        <f>CONCATENATE("insert import(clase, dep, actividad, meta, cate)values('",A2,"', '",B2,"', '",D2,"', '",E2,"', '",G2,"')")</f>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '020700', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1052,8 +1054,12 @@
       <c r="H3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I66" si="0">CONCATENATE("insert import(clase, dep, actividad, meta, cate)values('",A3,"', '",B3,"', '",D3,"', '",E3,"', '",G3,"')")</f>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '010000', '5000002', '0022', '9001')</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1078,8 +1084,12 @@
       <c r="H4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '010000', '5000002', '0022', '9001')</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1104,8 +1114,12 @@
       <c r="H5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '010002', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1130,8 +1144,12 @@
       <c r="H6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '010002', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1156,8 +1174,12 @@
       <c r="H7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '010100', '5000006', '0026', '9001')</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1182,8 +1204,12 @@
       <c r="H8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '010200', '5000001', '0021', '9001')</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1208,8 +1234,12 @@
       <c r="H9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '010300', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1234,8 +1264,12 @@
       <c r="H10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '010300', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1260,8 +1294,12 @@
       <c r="H11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '010400', '5000004', '0024', '9001')</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1286,8 +1324,12 @@
       <c r="H12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '010500', '5000002', '0022', '9001')</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1312,8 +1354,12 @@
       <c r="H13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '010600', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1338,8 +1384,12 @@
       <c r="H14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '010700', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -1364,8 +1414,12 @@
       <c r="H15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('M', '010700', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1390,8 +1444,12 @@
       <c r="H16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '010700', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1416,8 +1474,12 @@
       <c r="H17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '010800', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1442,8 +1504,12 @@
       <c r="H18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '010800', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1468,8 +1534,12 @@
       <c r="H19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '010900', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1494,8 +1564,12 @@
       <c r="H20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '010900', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1520,8 +1594,12 @@
       <c r="H21" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '010901', '5002189', '0031', '9002')</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1546,8 +1624,12 @@
       <c r="H22" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '010901', '5002189', '0031', '9002')</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1572,8 +1654,12 @@
       <c r="H23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '010902', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1598,8 +1684,12 @@
       <c r="H24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '010902', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1624,8 +1714,12 @@
       <c r="H25" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '011000', '5002006', '0030', '9002')</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1650,8 +1744,12 @@
       <c r="H26" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '011000', '5002006', '0030', '9002')</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1676,8 +1774,12 @@
       <c r="H27" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '011300', '5002267', '0032', '9002')</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -1702,8 +1804,12 @@
       <c r="H28" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '011300', '5002267', '0032', '9002')</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1728,8 +1834,12 @@
       <c r="H29" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '011400', '5002008', '0000', '9002')</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1754,8 +1864,12 @@
       <c r="H30" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '011400', '5002008', '0000', '9002')</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1780,8 +1894,12 @@
       <c r="H31" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '011500', '5001980', '0029', '9002')</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -1806,8 +1924,12 @@
       <c r="H32" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '011500', '5001980', '0029', '9002')</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -1832,8 +1954,12 @@
       <c r="H33" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '020000', '5000002', '0022', '9001')</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -1858,8 +1984,12 @@
       <c r="H34" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '020000', '5000002', '0022', '9001')</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1884,8 +2014,12 @@
       <c r="H35" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '020100', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>23</v>
       </c>
@@ -1910,8 +2044,12 @@
       <c r="H36" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '020100', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1936,8 +2074,12 @@
       <c r="H37" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '020200', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -1962,8 +2104,12 @@
       <c r="H38" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '020300', '5001792', '0028', '9002')</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -1988,8 +2134,12 @@
       <c r="H39" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '020300', '5001792', '0028', '9002')</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -2014,8 +2164,12 @@
       <c r="H40" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '020400', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>23</v>
       </c>
@@ -2040,8 +2194,12 @@
       <c r="H41" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '020400', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -2066,8 +2224,12 @@
       <c r="H42" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '020500', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -2092,8 +2254,12 @@
       <c r="H43" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '020500', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -2118,8 +2284,12 @@
       <c r="H44" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '020600', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -2144,8 +2314,12 @@
       <c r="H45" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="I45" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '020600', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -2170,8 +2344,12 @@
       <c r="H46" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="I46" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '030100', '5000005', '0025', '9001')</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -2196,8 +2374,12 @@
       <c r="H47" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '030200', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -2222,8 +2404,12 @@
       <c r="H48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="I48" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '030300', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>23</v>
       </c>
@@ -2248,8 +2434,12 @@
       <c r="H49" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="I49" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '030300', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -2274,8 +2464,12 @@
       <c r="H50" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '030500', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -2300,8 +2494,12 @@
       <c r="H51" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="I51" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '030500', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -2326,8 +2524,12 @@
       <c r="H52" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="I52" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '700000', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -2352,8 +2554,12 @@
       <c r="H53" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="I53" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '040000', '5000002', '0022', '9001')</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>23</v>
       </c>
@@ -2378,8 +2584,12 @@
       <c r="H54" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="55" spans="1:8">
+      <c r="I54" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '040000', '5000002', '0022', '9001')</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -2404,8 +2614,12 @@
       <c r="H55" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="56" spans="1:8">
+      <c r="I55" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '050000', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -2430,8 +2644,12 @@
       <c r="H56" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="I56" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '060000', '5001792', '0028', '9001')</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -2456,8 +2674,12 @@
       <c r="H57" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="58" spans="1:8">
+      <c r="I57" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '100000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -2482,8 +2704,12 @@
       <c r="H58" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="I58" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '100000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>23</v>
       </c>
@@ -2508,8 +2734,12 @@
       <c r="H59" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="I59" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '110000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -2534,8 +2764,12 @@
       <c r="H60" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="61" spans="1:8">
+      <c r="I60" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '110000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>23</v>
       </c>
@@ -2560,8 +2794,12 @@
       <c r="H61" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="62" spans="1:8">
+      <c r="I61" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '120000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -2586,8 +2824,12 @@
       <c r="H62" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="I62" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '120000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>23</v>
       </c>
@@ -2612,8 +2854,12 @@
       <c r="H63" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="I63" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '130000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -2638,8 +2884,12 @@
       <c r="H64" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="65" spans="1:8">
+      <c r="I64" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '130000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>23</v>
       </c>
@@ -2664,8 +2914,12 @@
       <c r="H65" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="I65" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '140000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -2690,8 +2944,12 @@
       <c r="H66" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="I66" t="str">
+        <f t="shared" si="0"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '140000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>23</v>
       </c>
@@ -2716,8 +2974,12 @@
       <c r="H67" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="68" spans="1:8">
+      <c r="I67" t="str">
+        <f t="shared" ref="I67:I96" si="1">CONCATENATE("insert import(clase, dep, actividad, meta, cate)values('",A67,"', '",B67,"', '",D67,"', '",E67,"', '",G67,"')")</f>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '150000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -2742,8 +3004,12 @@
       <c r="H68" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="I68" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '150000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>23</v>
       </c>
@@ -2768,8 +3034,12 @@
       <c r="H69" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="70" spans="1:8">
+      <c r="I69" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '160000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -2794,8 +3064,12 @@
       <c r="H70" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="71" spans="1:8">
+      <c r="I70" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '160000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>23</v>
       </c>
@@ -2820,8 +3094,12 @@
       <c r="H71" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="72" spans="1:8">
+      <c r="I71" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '170000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -2846,8 +3124,12 @@
       <c r="H72" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="73" spans="1:8">
+      <c r="I72" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '170000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>23</v>
       </c>
@@ -2872,8 +3154,12 @@
       <c r="H73" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="74" spans="1:8">
+      <c r="I73" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '180000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -2898,8 +3184,12 @@
       <c r="H74" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="75" spans="1:8">
+      <c r="I74" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '180000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>23</v>
       </c>
@@ -2924,8 +3214,12 @@
       <c r="H75" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="76" spans="1:8">
+      <c r="I75" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '190000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -2950,8 +3244,12 @@
       <c r="H76" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="77" spans="1:8">
+      <c r="I76" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '190000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>23</v>
       </c>
@@ -2976,8 +3274,12 @@
       <c r="H77" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="78" spans="1:8">
+      <c r="I77" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '200000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -3002,8 +3304,12 @@
       <c r="H78" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="79" spans="1:8">
+      <c r="I78" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '200000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -3028,8 +3334,12 @@
       <c r="H79" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="80" spans="1:8">
+      <c r="I79" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '210000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>8</v>
       </c>
@@ -3054,8 +3364,12 @@
       <c r="H80" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="81" spans="1:8">
+      <c r="I80" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '210000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>23</v>
       </c>
@@ -3080,8 +3394,12 @@
       <c r="H81" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="82" spans="1:8">
+      <c r="I81" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '220000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>8</v>
       </c>
@@ -3106,8 +3424,12 @@
       <c r="H82" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="83" spans="1:8">
+      <c r="I82" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '220000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>23</v>
       </c>
@@ -3132,8 +3454,12 @@
       <c r="H83" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="84" spans="1:8">
+      <c r="I83" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '230000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -3158,8 +3484,12 @@
       <c r="H84" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="85" spans="1:8">
+      <c r="I84" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '230000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>23</v>
       </c>
@@ -3184,8 +3514,12 @@
       <c r="H85" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="86" spans="1:8">
+      <c r="I85" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '240000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -3210,8 +3544,12 @@
       <c r="H86" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="87" spans="1:8">
+      <c r="I86" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '240000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>23</v>
       </c>
@@ -3236,8 +3574,12 @@
       <c r="H87" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="88" spans="1:8">
+      <c r="I87" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '250000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>8</v>
       </c>
@@ -3262,8 +3604,12 @@
       <c r="H88" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="89" spans="1:8">
+      <c r="I88" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '250000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>23</v>
       </c>
@@ -3288,8 +3634,12 @@
       <c r="H89" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="90" spans="1:8">
+      <c r="I89" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '260000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>8</v>
       </c>
@@ -3314,8 +3664,12 @@
       <c r="H90" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="91" spans="1:8">
+      <c r="I90" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '260000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>54</v>
       </c>
@@ -3340,8 +3694,12 @@
       <c r="H91" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="92" spans="1:8">
+      <c r="I91" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('M', '260000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>23</v>
       </c>
@@ -3366,8 +3724,12 @@
       <c r="H92" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="93" spans="1:8">
+      <c r="I92" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '270000', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -3392,8 +3754,12 @@
       <c r="H93" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="94" spans="1:8">
+      <c r="I93" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '270000', '5000276', '0011', '0066')</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>8</v>
       </c>
@@ -3418,8 +3784,12 @@
       <c r="H94" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="95" spans="1:8">
+      <c r="I94" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('A', '041000', '5000003', '0023', '9001')</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>23</v>
       </c>
@@ -3444,8 +3814,12 @@
       <c r="H95" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="96" spans="1:8">
+      <c r="I95" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '020200', '5005857', '0014', '0066')</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>23</v>
       </c>
@@ -3469,6 +3843,10 @@
       </c>
       <c r="H96" t="s">
         <v>15</v>
+      </c>
+      <c r="I96" t="str">
+        <f t="shared" si="1"/>
+        <v>insert import(clase, dep, actividad, meta, cate)values('D', '010001', '5000002', '0022', '0066')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>